<commit_message>
Conversion parameters to Excel
</commit_message>
<xml_diff>
--- a/Data/transport_parameters.xlsx
+++ b/Data/transport_parameters.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="8_{465E32D3-D5CA-4EAD-9512-3B08779BE17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AC085BE-C997-47D3-B6CB-8D472AB345C8}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12405" activeTab="3" xr2:uid="{01CAD706-003C-4A74-9F03-CC297AE4FC2E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{01CAD706-003C-4A74-9F03-CC297AE4FC2E}"/>
   </bookViews>
   <sheets>
     <sheet name="500 bar" sheetId="1" r:id="rId1"/>
@@ -444,17 +444,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,7 +462,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -470,7 +470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -478,7 +478,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -486,7 +486,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -494,7 +494,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -502,7 +502,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -510,7 +510,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -518,7 +518,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -526,7 +526,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -542,7 +542,7 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -550,7 +550,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -558,7 +558,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -566,7 +566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -584,20 +584,20 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -605,7 +605,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -613,7 +613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -621,7 +621,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -629,7 +629,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -637,7 +637,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -645,7 +645,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -653,7 +653,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -661,7 +661,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -669,7 +669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -677,7 +677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -685,7 +685,7 @@
         <v>860000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -701,7 +701,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -709,7 +709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -727,20 +727,20 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -748,7 +748,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -756,7 +756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -764,7 +764,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -772,7 +772,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -780,7 +780,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -788,7 +788,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -796,7 +796,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -804,7 +804,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -812,7 +812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -820,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -828,7 +828,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -844,7 +844,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -852,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -870,20 +870,20 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -891,7 +891,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -899,7 +899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -907,7 +907,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -915,7 +915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -923,7 +923,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -939,7 +939,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -947,7 +947,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -955,7 +955,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -963,7 +963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -971,7 +971,7 @@
         <v>190000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -979,7 +979,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -987,7 +987,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -995,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>